<commit_message>
got daily accounts working, and compiling backend in daily script
</commit_message>
<xml_diff>
--- a/Phase6/DefectReport.xlsx
+++ b/Phase6/DefectReport.xlsx
@@ -66,9 +66,15 @@
       <left style="none">
         <color rgb="FFC7C7C7"/>
       </left>
+      <right style="none">
+        <color rgb="FFC7C7C7"/>
+      </right>
       <top style="none">
         <color rgb="FFC7C7C7"/>
       </top>
+      <bottom style="none">
+        <color rgb="FFC7C7C7"/>
+      </bottom>
     </border>
     <border diagonalUp="0" diagonalDown="0">
       <left style="none">
@@ -117,13 +123,14 @@
   <dimension ref="A1:XFD49"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="85" tabSelected="1">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" style="1" width="66.88674" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" style="1" width="57.28227" customWidth="1"/>
+    <col min="2" max="2" style="1" width="57.28227" customWidth="1"/>
+    <col min="3" max="3" style="1" width="75.62571" customWidth="1"/>
     <col min="4" max="16384" style="1"/>
   </cols>
   <sheetData>
@@ -16525,9 +16532,11 @@
 what():  stod</v>
       </c>
       <c r="B2" s="3" t="str">
-        <v>Deposit from I/O redirection can cause given error</v>
+        <v>Deposit from I/O redirection caused given error</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3" t="str">
+        <v>The session file was incorrectly formatted (didn't include deposit amount)</v>
+      </c>
     </row>
     <row r="3" spans="1:16384">
       <c r="A3" s="3"/>

</xml_diff>

<commit_message>
Provided adatper from Front End output to Back End input
</commit_message>
<xml_diff>
--- a/Phase6/DefectReport.xlsx
+++ b/Phase6/DefectReport.xlsx
@@ -29,7 +29,6 @@
   <fonts count="3">
     <font>
       <i val="0"/>
-      <color rgb="FF000000"/>
       <name val="Sans"/>
       <strike val="0"/>
     </font>
@@ -50,28 +49,22 @@
       <strike val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill/>
-    </fill>
   </fills>
   <borders count="2">
-    <border>
+    <border diagonalDown="0">
       <left style="none">
         <color rgb="FFC7C7C7"/>
       </left>
       <right style="none">
         <color rgb="FFC7C7C7"/>
       </right>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
       <bottom style="none">
         <color rgb="FFC7C7C7"/>
       </bottom>
@@ -92,10 +85,10 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="2" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf applyAlignment="0" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
+    <xf applyAlignment="0" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
@@ -123,13 +116,13 @@
   <dimension ref="A1:XFD49"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="85" tabSelected="1">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" style="1" width="66.88674" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" style="1" width="57.28227" customWidth="1"/>
+    <col min="2" max="2" style="1" width="61.67697" customWidth="1"/>
     <col min="3" max="3" style="1" width="75.62571" customWidth="1"/>
     <col min="4" max="16384" style="1"/>
   </cols>
@@ -16539,23 +16532,41 @@
       </c>
     </row>
     <row r="3" spans="1:16384">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="3" t="str">
+        <v>Backend and Frontend use different account transaction format</v>
+      </c>
+      <c r="B3" s="3" t="str">
+        <v>The Backend uses spaces, and the Frontend uses underscores</v>
+      </c>
+      <c r="C3" s="3" t="str">
+        <v>Updated the Backend to read in input files with underscores</v>
+      </c>
     </row>
     <row r="4" spans="1:16384">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="str">
+        <v>Backend expects login transaction?</v>
+      </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:16384">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="A5" s="3" t="str">
+        <v>Frontend has END_OF_FILE line in user accounts</v>
+      </c>
+      <c r="B5" s="3" t="str">
+        <v>Backend not expecting 00000_END_OF_FILE____________00000.00</v>
+      </c>
+      <c r="C5" s="3" t="str">
+        <v>Provide adapter to remove line</v>
+      </c>
     </row>
     <row r="6" spans="1:16384">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="3" t="str">
+        <v>FrontEnd file output does match Backend file input</v>
+      </c>
+      <c r="B6" s="3" t="str">
+        <v>Front end user accounts doesn't match the back end expected input for user accounts</v>
+      </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:16384">

</xml_diff>

<commit_message>
Continued on daily.sh, and resolving defects
</commit_message>
<xml_diff>
--- a/Phase6/DefectReport.xlsx
+++ b/Phase6/DefectReport.xlsx
@@ -22,6 +22,20 @@
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <webPublishing allowPng="1" css="0" codePage="1252"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3" count="3">
+  <si>
+    <t>Backend and Frontend use different account transaction format (transactions)</t>
+  </si>
+  <si>
+    <t>The Backend uses spaces, and the Frontend uses underscores</t>
+  </si>
+  <si>
+    <t>Updated the Backend to read in input files with underscores</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -116,7 +130,7 @@
   <dimension ref="A1:XFD49"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="85" tabSelected="1">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -16532,14 +16546,14 @@
       </c>
     </row>
     <row r="3" spans="1:16384">
-      <c r="A3" s="3" t="str">
-        <v>Backend and Frontend use different account transaction format</v>
+      <c r="A3" s="3" t="s">
+        <v>0</v>
       </c>
-      <c r="B3" s="3" t="str">
-        <v>The Backend uses spaces, and the Frontend uses underscores</v>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
       </c>
-      <c r="C3" s="3" t="str">
-        <v>Updated the Backend to read in input files with underscores</v>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:16384">
@@ -16562,16 +16576,22 @@
     </row>
     <row r="6" spans="1:16384">
       <c r="A6" s="3" t="str">
-        <v>FrontEnd file output does match Backend file input</v>
+        <v>FrontEnd file output does match Backend file input 2</v>
       </c>
       <c r="B6" s="3" t="str">
-        <v>Front end user accounts doesn't match the back end expected input for user accounts</v>
+        <v>Frontend doesn't have N or S on user accounts</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3" t="str">
+        <v>added to look like: 00001_John_Doe_____________A_00050.00_N</v>
+      </c>
     </row>
     <row r="7" spans="1:16384">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="3" t="str">
+        <v>Backend and Frontend use different account transaction format (accounts)</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:16384">

</xml_diff>